<commit_message>
revision resultados tatara, anotando en antecedentes mientras se procesa sensibilidad genesis en el otro pc
</commit_message>
<xml_diff>
--- a/Proyectos Evaluados/Tatara/Antecedentes PF - Tatara_V2.xlsx
+++ b/Proyectos Evaluados/Tatara/Antecedentes PF - Tatara_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano Chaura\Desktop\ejecucion-modelos\Proyectos Evaluados\Tatara\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D22D314-8EAE-4A5E-9B74-B19A6640C582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17023B62-BB41-4F30-AD73-AA67444526B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="2" activeTab="4" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Caso BESS" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="70">
   <si>
     <t>Nodo de Referencia (DNV)</t>
   </si>
@@ -251,16 +251,165 @@
     <t>30 MW 180 MWh (6 hrs)</t>
   </si>
   <si>
-    <t xml:space="preserve">PV 30 MWp, BESS 30 MW 120 MWh </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 27 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 90 MWh  (3 hrs)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">PV 27 MWp, BESS 30 MW 90 MWh </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 27 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 120 MWh (4 hrs)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">PV 27 MWp, BESS 30 MW 120 MWh </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 27 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 150 MWh (5 hrs)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">PV 27 MWp, BESS 30 MW 150 MWh </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 30 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 90 MWh (3 hrs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 30 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 120 MWh (4 hrs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 30 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 150 MWh (5 hrs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PV 33 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 90 MWh  (3 hrs)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PV 33 MWp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, BESS 30 MW 90 MWh  (3 hrs)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -482,7 +631,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,6 +726,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1603,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD17015-A551-4C2B-85B3-9418ADFEA835}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72059,10 +72214,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72286,71 +72441,153 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="18">
-        <v>9.3200000000000005E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="D14" s="18">
-        <v>0.1002</v>
+        <v>0.1031</v>
       </c>
       <c r="E14" s="17">
-        <v>8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F14" s="17">
         <v>7.9</v>
       </c>
       <c r="G14" s="17">
-        <v>61.6</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="16">
-        <v>9.5799999999999996E-2</v>
+        <v>9.9699999999999997E-2</v>
       </c>
       <c r="D15" s="16">
-        <v>0.1027</v>
+        <v>0.1062</v>
       </c>
       <c r="E15" s="15">
-        <v>9.56</v>
+        <v>10.7</v>
       </c>
       <c r="F15" s="15">
         <v>7.6</v>
       </c>
       <c r="G15" s="15">
-        <v>70.099999999999994</v>
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="C16" s="18">
+        <v>9.4299999999999995E-2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.1012</v>
+      </c>
+      <c r="E16" s="17">
+        <v>10.1</v>
+      </c>
+      <c r="F16" s="17">
+        <v>7.8</v>
+      </c>
+      <c r="G16" s="17">
+        <v>76.5</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.10059999999999999</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.1074</v>
+      </c>
+      <c r="E17" s="15">
+        <v>10.82</v>
+      </c>
+      <c r="F17" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="G17" s="15">
+        <v>52.6</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="B18" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.1002</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.1067</v>
+      </c>
+      <c r="E18" s="17">
+        <v>11.5</v>
+      </c>
+      <c r="F18" s="17">
+        <v>7.66</v>
+      </c>
+      <c r="G18" s="17">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="16">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.1032</v>
+      </c>
+      <c r="E19" s="15">
+        <v>11.38</v>
+      </c>
+      <c r="F19" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="G19" s="15">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -72358,15 +72595,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9973b7cd-78b1-41ec-8b66-6143e90e5574" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="3b9b9037-28f8-4200-a961-13fb81bc61ed" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b9b9037-28f8-4200-a961-13fb81bc61ed">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -72631,21 +72865,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9973b7cd-78b1-41ec-8b66-6143e90e5574" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="3b9b9037-28f8-4200-a961-13fb81bc61ed" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b9b9037-28f8-4200-a961-13fb81bc61ed">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D6E3B29-6441-466D-950A-CE8D2F0401D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC21C0BF-6CEF-427E-B508-C77C090066B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9973b7cd-78b1-41ec-8b66-6143e90e5574"/>
-    <ds:schemaRef ds:uri="3b9b9037-28f8-4200-a961-13fb81bc61ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -72670,9 +72904,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC21C0BF-6CEF-427E-B508-C77C090066B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D6E3B29-6441-466D-950A-CE8D2F0401D8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9973b7cd-78b1-41ec-8b66-6143e90e5574"/>
+    <ds:schemaRef ds:uri="3b9b9037-28f8-4200-a961-13fb81bc61ed"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>